<commit_message>
Fixed plot saving bug
</commit_message>
<xml_diff>
--- a/Spreadsheets/5600X.xlsx
+++ b/Spreadsheets/5600X.xlsx
@@ -6877,7 +6877,7 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B202" t="inlineStr">
         <is>
@@ -6909,7 +6909,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B203" t="inlineStr">
         <is>
@@ -6941,7 +6941,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B204" t="inlineStr">
         <is>
@@ -6973,7 +6973,7 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B205" t="inlineStr">
         <is>
@@ -7005,7 +7005,7 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B206" t="inlineStr">
         <is>
@@ -7037,7 +7037,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B207" t="inlineStr">
         <is>
@@ -7069,7 +7069,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B208" t="inlineStr">
         <is>
@@ -7101,7 +7101,7 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B209" t="inlineStr">
         <is>
@@ -7133,7 +7133,7 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B210" t="inlineStr">
         <is>
@@ -7165,7 +7165,7 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B211" t="inlineStr">
         <is>
@@ -7197,7 +7197,7 @@
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B212" t="inlineStr">
         <is>
@@ -7229,7 +7229,7 @@
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B213" t="inlineStr">
         <is>
@@ -7261,7 +7261,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B214" t="inlineStr">
         <is>
@@ -7293,7 +7293,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B215" t="inlineStr">
         <is>
@@ -7325,7 +7325,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B216" t="inlineStr">
         <is>
@@ -7357,7 +7357,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B217" t="inlineStr">
         <is>
@@ -7389,7 +7389,7 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B218" t="inlineStr">
         <is>
@@ -7421,7 +7421,7 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B219" t="inlineStr">
         <is>
@@ -7453,7 +7453,7 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B220" t="inlineStr">
         <is>
@@ -7485,7 +7485,7 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B221" t="inlineStr">
         <is>
@@ -7517,7 +7517,7 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B222" t="inlineStr">
         <is>
@@ -7549,7 +7549,7 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B223" t="inlineStr">
         <is>
@@ -7581,7 +7581,7 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B224" t="inlineStr">
         <is>
@@ -7613,7 +7613,7 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B225" t="inlineStr">
         <is>
@@ -7645,7 +7645,7 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B226" t="inlineStr">
         <is>
@@ -7677,7 +7677,7 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B227" t="inlineStr">
         <is>
@@ -7709,7 +7709,7 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B228" t="inlineStr">
         <is>
@@ -7741,7 +7741,7 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B229" t="inlineStr">
         <is>
@@ -7773,7 +7773,7 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B230" t="inlineStr">
         <is>
@@ -7805,7 +7805,7 @@
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B231" t="inlineStr">
         <is>
@@ -7837,7 +7837,7 @@
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B232" t="inlineStr">
         <is>
@@ -7869,7 +7869,7 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B233" t="inlineStr">
         <is>
@@ -7901,7 +7901,7 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B234" t="inlineStr">
         <is>
@@ -7933,7 +7933,7 @@
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B235" t="inlineStr">
         <is>
@@ -7965,7 +7965,7 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B236" t="inlineStr">
         <is>
@@ -7997,7 +7997,7 @@
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B237" t="inlineStr">
         <is>
@@ -8029,7 +8029,7 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B238" t="inlineStr">
         <is>
@@ -8061,7 +8061,7 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B239" t="inlineStr">
         <is>
@@ -8093,7 +8093,7 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B240" t="inlineStr">
         <is>
@@ -8125,7 +8125,7 @@
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B241" t="inlineStr">
         <is>
@@ -8157,11 +8157,11 @@
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>AMD Ryzen 5 5600X Desktop Processor, IN HAND❤️, WHO WILL BE LUCKY?!?</t>
+          <t>AMD Ryzen 5 5600X Desktop Processor, IN HAND❤��, WHO WILL BE LUCKY?!?</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -8189,7 +8189,7 @@
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B243" t="inlineStr">
         <is>
@@ -8221,7 +8221,7 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B244" t="inlineStr">
         <is>
@@ -8253,7 +8253,7 @@
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B245" t="inlineStr">
         <is>
@@ -8285,7 +8285,7 @@
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B246" t="inlineStr">
         <is>
@@ -8317,7 +8317,7 @@
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B247" t="inlineStr">
         <is>
@@ -8349,7 +8349,7 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B248" t="inlineStr">
         <is>
@@ -8381,7 +8381,7 @@
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B249" t="inlineStr">
         <is>
@@ -8413,7 +8413,7 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B250" t="inlineStr">
         <is>
@@ -8445,7 +8445,7 @@
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B251" t="inlineStr">
         <is>
@@ -8477,7 +8477,7 @@
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B252" t="inlineStr">
         <is>
@@ -8509,7 +8509,7 @@
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B253" t="inlineStr">
         <is>
@@ -8541,7 +8541,7 @@
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B254" t="inlineStr">
         <is>
@@ -8573,7 +8573,7 @@
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B255" t="inlineStr">
         <is>
@@ -8605,7 +8605,7 @@
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B256" t="inlineStr">
         <is>
@@ -8637,7 +8637,7 @@
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B257" t="inlineStr">
         <is>
@@ -8669,7 +8669,7 @@
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B258" t="inlineStr">
         <is>
@@ -8701,7 +8701,7 @@
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B259" t="inlineStr">
         <is>
@@ -8733,7 +8733,7 @@
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B260" t="inlineStr">
         <is>
@@ -8765,7 +8765,7 @@
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B261" t="inlineStr">
         <is>
@@ -8797,7 +8797,7 @@
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B262" t="inlineStr">
         <is>
@@ -8829,7 +8829,7 @@
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B263" t="inlineStr">
         <is>
@@ -8861,7 +8861,7 @@
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B264" t="inlineStr">
         <is>
@@ -8893,7 +8893,7 @@
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B265" t="inlineStr">
         <is>
@@ -8925,7 +8925,7 @@
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B266" t="inlineStr">
         <is>
@@ -8957,7 +8957,7 @@
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B267" t="inlineStr">
         <is>
@@ -8989,7 +8989,7 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B268" t="inlineStr">
         <is>
@@ -9021,7 +9021,7 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B269" t="inlineStr">
         <is>
@@ -9053,7 +9053,7 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B270" t="inlineStr">
         <is>
@@ -9085,7 +9085,7 @@
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B271" t="inlineStr">
         <is>
@@ -9117,7 +9117,7 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B272" t="inlineStr">
         <is>
@@ -9149,7 +9149,7 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B273" t="inlineStr">
         <is>
@@ -9181,7 +9181,7 @@
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B274" t="inlineStr">
         <is>
@@ -9213,7 +9213,7 @@
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B275" t="inlineStr">
         <is>
@@ -9245,7 +9245,7 @@
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B276" t="inlineStr">
         <is>
@@ -9277,7 +9277,7 @@
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B277" t="inlineStr">
         <is>
@@ -9309,7 +9309,7 @@
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B278" t="inlineStr">
         <is>
@@ -9341,7 +9341,7 @@
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B279" t="inlineStr">
         <is>
@@ -9373,7 +9373,7 @@
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B280" t="inlineStr">
         <is>
@@ -9405,7 +9405,7 @@
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B281" t="inlineStr">
         <is>
@@ -9437,7 +9437,7 @@
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B282" t="inlineStr">
         <is>
@@ -9469,7 +9469,7 @@
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B283" t="inlineStr">
         <is>
@@ -9501,7 +9501,7 @@
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B284" t="inlineStr">
         <is>
@@ -9533,7 +9533,7 @@
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B285" t="inlineStr">
         <is>
@@ -9565,7 +9565,7 @@
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B286" t="inlineStr">
         <is>
@@ -9597,7 +9597,7 @@
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B287" t="inlineStr">
         <is>
@@ -9629,7 +9629,7 @@
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B288" t="inlineStr">
         <is>
@@ -9661,7 +9661,7 @@
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B289" t="inlineStr">
         <is>
@@ -9693,7 +9693,7 @@
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B290" t="inlineStr">
         <is>
@@ -9725,7 +9725,7 @@
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B291" t="inlineStr">
         <is>
@@ -9757,7 +9757,7 @@
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B292" t="inlineStr">
         <is>
@@ -9789,7 +9789,7 @@
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B293" t="inlineStr">
         <is>
@@ -9821,7 +9821,7 @@
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B294" t="inlineStr">
         <is>
@@ -9853,7 +9853,7 @@
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B295" t="inlineStr">
         <is>
@@ -9885,7 +9885,7 @@
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B296" t="inlineStr">
         <is>
@@ -9917,7 +9917,7 @@
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B297" t="inlineStr">
         <is>
@@ -9949,7 +9949,7 @@
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B298" t="inlineStr">
         <is>
@@ -9981,7 +9981,7 @@
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B299" t="inlineStr">
         <is>
@@ -10013,7 +10013,7 @@
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B300" t="inlineStr">
         <is>
@@ -10045,7 +10045,7 @@
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B301" t="inlineStr">
         <is>
@@ -10077,7 +10077,7 @@
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B302" t="inlineStr">
         <is>
@@ -10109,7 +10109,7 @@
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B303" t="inlineStr">
         <is>
@@ -10141,7 +10141,7 @@
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B304" t="inlineStr">
         <is>
@@ -10173,7 +10173,7 @@
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B305" t="inlineStr">
         <is>
@@ -10205,7 +10205,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B306" t="inlineStr">
         <is>
@@ -10237,7 +10237,7 @@
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B307" t="inlineStr">
         <is>
@@ -10269,7 +10269,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B308" t="inlineStr">
         <is>
@@ -10301,7 +10301,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B309" t="inlineStr">
         <is>
@@ -10333,7 +10333,7 @@
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B310" t="inlineStr">
         <is>
@@ -10365,7 +10365,7 @@
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B311" t="inlineStr">
         <is>
@@ -10397,7 +10397,7 @@
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B312" t="inlineStr">
         <is>
@@ -10429,7 +10429,7 @@
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B313" t="inlineStr">
         <is>
@@ -10461,7 +10461,7 @@
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B314" t="inlineStr">
         <is>
@@ -10493,7 +10493,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B315" t="inlineStr">
         <is>
@@ -10525,7 +10525,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B316" t="inlineStr">
         <is>
@@ -10557,7 +10557,7 @@
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B317" t="inlineStr">
         <is>
@@ -10589,7 +10589,7 @@
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B318" t="inlineStr">
         <is>
@@ -10621,7 +10621,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B319" t="inlineStr">
         <is>
@@ -10653,7 +10653,7 @@
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B320" t="inlineStr">
         <is>
@@ -10685,7 +10685,7 @@
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B321" t="inlineStr">
         <is>
@@ -10717,7 +10717,7 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B322" t="inlineStr">
         <is>
@@ -10749,7 +10749,7 @@
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B323" t="inlineStr">
         <is>
@@ -10781,7 +10781,7 @@
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B324" t="inlineStr">
         <is>
@@ -10813,7 +10813,7 @@
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B325" t="inlineStr">
         <is>
@@ -10845,7 +10845,7 @@
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B326" t="inlineStr">
         <is>
@@ -10877,7 +10877,7 @@
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B327" t="inlineStr">
         <is>
@@ -10909,7 +10909,7 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B328" t="inlineStr">
         <is>
@@ -10941,7 +10941,7 @@
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B329" t="inlineStr">
         <is>
@@ -10973,7 +10973,7 @@
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B330" t="inlineStr">
         <is>
@@ -11005,7 +11005,7 @@
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B331" t="inlineStr">
         <is>
@@ -11037,7 +11037,7 @@
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B332" t="inlineStr">
         <is>
@@ -11069,7 +11069,7 @@
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B333" t="inlineStr">
         <is>
@@ -11101,7 +11101,7 @@
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B334" t="inlineStr">
         <is>
@@ -11133,7 +11133,7 @@
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B335" t="inlineStr">
         <is>
@@ -11165,7 +11165,7 @@
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B336" t="inlineStr">
         <is>
@@ -11197,7 +11197,7 @@
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B337" t="inlineStr">
         <is>
@@ -11229,7 +11229,7 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B338" t="inlineStr">
         <is>
@@ -11261,7 +11261,7 @@
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B339" t="inlineStr">
         <is>
@@ -11293,7 +11293,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B340" t="inlineStr">
         <is>
@@ -11325,7 +11325,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B341" t="inlineStr">
         <is>
@@ -11357,7 +11357,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B342" t="inlineStr">
         <is>
@@ -11389,7 +11389,7 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B343" t="inlineStr">
         <is>
@@ -11421,7 +11421,7 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B344" t="inlineStr">
         <is>
@@ -11453,7 +11453,7 @@
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B345" t="inlineStr">
         <is>
@@ -11485,7 +11485,7 @@
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B346" t="inlineStr">
         <is>
@@ -11517,7 +11517,7 @@
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B347" t="inlineStr">
         <is>
@@ -11549,7 +11549,7 @@
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B348" t="inlineStr">
         <is>
@@ -11581,7 +11581,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B349" t="inlineStr">
         <is>
@@ -11613,7 +11613,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B350" t="inlineStr">
         <is>
@@ -11645,7 +11645,7 @@
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B351" t="inlineStr">
         <is>
@@ -11677,7 +11677,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B352" t="inlineStr">
         <is>
@@ -11709,7 +11709,7 @@
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B353" t="inlineStr">
         <is>
@@ -11741,7 +11741,7 @@
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B354" t="inlineStr">
         <is>
@@ -11773,7 +11773,7 @@
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B355" t="inlineStr">
         <is>
@@ -11805,7 +11805,7 @@
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B356" t="inlineStr">
         <is>
@@ -11837,7 +11837,7 @@
     </row>
     <row r="357">
       <c r="A357" s="1" t="n">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B357" t="inlineStr">
         <is>
@@ -11869,7 +11869,7 @@
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B358" t="inlineStr">
         <is>
@@ -11901,7 +11901,7 @@
     </row>
     <row r="359">
       <c r="A359" s="1" t="n">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B359" t="inlineStr">
         <is>
@@ -11933,7 +11933,7 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B360" t="inlineStr">
         <is>
@@ -11965,7 +11965,7 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B361" t="inlineStr">
         <is>
@@ -11997,7 +11997,7 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="n">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B362" t="inlineStr">
         <is>
@@ -12029,7 +12029,7 @@
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B363" t="inlineStr">
         <is>
@@ -12061,7 +12061,7 @@
     </row>
     <row r="364">
       <c r="A364" s="1" t="n">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B364" t="inlineStr">
         <is>
@@ -12093,7 +12093,7 @@
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B365" t="inlineStr">
         <is>
@@ -12125,7 +12125,7 @@
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B366" t="inlineStr">
         <is>
@@ -12157,7 +12157,7 @@
     </row>
     <row r="367">
       <c r="A367" s="1" t="n">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B367" t="inlineStr">
         <is>
@@ -12189,7 +12189,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B368" t="inlineStr">
         <is>
@@ -12221,7 +12221,7 @@
     </row>
     <row r="369">
       <c r="A369" s="1" t="n">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B369" t="inlineStr">
         <is>
@@ -12253,7 +12253,7 @@
     </row>
     <row r="370">
       <c r="A370" s="1" t="n">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B370" t="inlineStr">
         <is>
@@ -12285,7 +12285,7 @@
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B371" t="inlineStr">
         <is>
@@ -12317,7 +12317,7 @@
     </row>
     <row r="372">
       <c r="A372" s="1" t="n">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B372" t="inlineStr">
         <is>
@@ -12349,7 +12349,7 @@
     </row>
     <row r="373">
       <c r="A373" s="1" t="n">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B373" t="inlineStr">
         <is>
@@ -12381,7 +12381,7 @@
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B374" t="inlineStr">
         <is>
@@ -12413,7 +12413,7 @@
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B375" t="inlineStr">
         <is>
@@ -12445,7 +12445,7 @@
     </row>
     <row r="376">
       <c r="A376" s="1" t="n">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B376" t="inlineStr">
         <is>
@@ -12477,7 +12477,7 @@
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B377" t="inlineStr">
         <is>
@@ -12509,7 +12509,7 @@
     </row>
     <row r="378">
       <c r="A378" s="1" t="n">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B378" t="inlineStr">
         <is>
@@ -12541,7 +12541,7 @@
     </row>
     <row r="379">
       <c r="A379" s="1" t="n">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B379" t="inlineStr">
         <is>
@@ -12573,7 +12573,7 @@
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B380" t="inlineStr">
         <is>
@@ -12605,7 +12605,7 @@
     </row>
     <row r="381">
       <c r="A381" s="1" t="n">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B381" t="inlineStr">
         <is>
@@ -12637,7 +12637,7 @@
     </row>
     <row r="382">
       <c r="A382" s="1" t="n">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B382" t="inlineStr">
         <is>
@@ -12669,7 +12669,7 @@
     </row>
     <row r="383">
       <c r="A383" s="1" t="n">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B383" t="inlineStr">
         <is>
@@ -12701,7 +12701,7 @@
     </row>
     <row r="384">
       <c r="A384" s="1" t="n">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B384" t="inlineStr">
         <is>
@@ -12733,7 +12733,7 @@
     </row>
     <row r="385">
       <c r="A385" s="1" t="n">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B385" t="inlineStr">
         <is>
@@ -12765,7 +12765,7 @@
     </row>
     <row r="386">
       <c r="A386" s="1" t="n">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B386" t="inlineStr">
         <is>
@@ -12797,7 +12797,7 @@
     </row>
     <row r="387">
       <c r="A387" s="1" t="n">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B387" t="inlineStr">
         <is>
@@ -12829,7 +12829,7 @@
     </row>
     <row r="388">
       <c r="A388" s="1" t="n">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B388" t="inlineStr">
         <is>
@@ -12861,7 +12861,7 @@
     </row>
     <row r="389">
       <c r="A389" s="1" t="n">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B389" t="inlineStr">
         <is>
@@ -12893,7 +12893,7 @@
     </row>
     <row r="390">
       <c r="A390" s="1" t="n">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B390" t="inlineStr">
         <is>
@@ -12925,7 +12925,7 @@
     </row>
     <row r="391">
       <c r="A391" s="1" t="n">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B391" t="inlineStr">
         <is>
@@ -12957,7 +12957,7 @@
     </row>
     <row r="392">
       <c r="A392" s="1" t="n">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B392" t="inlineStr">
         <is>
@@ -12989,7 +12989,7 @@
     </row>
     <row r="393">
       <c r="A393" s="1" t="n">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B393" t="inlineStr">
         <is>
@@ -13021,7 +13021,7 @@
     </row>
     <row r="394">
       <c r="A394" s="1" t="n">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B394" t="inlineStr">
         <is>
@@ -13053,7 +13053,7 @@
     </row>
     <row r="395">
       <c r="A395" s="1" t="n">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B395" t="inlineStr">
         <is>
@@ -13085,7 +13085,7 @@
     </row>
     <row r="396">
       <c r="A396" s="1" t="n">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B396" t="inlineStr">
         <is>
@@ -13117,7 +13117,7 @@
     </row>
     <row r="397">
       <c r="A397" s="1" t="n">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B397" t="inlineStr">
         <is>
@@ -13149,7 +13149,7 @@
     </row>
     <row r="398">
       <c r="A398" s="1" t="n">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B398" t="inlineStr">
         <is>
@@ -13181,7 +13181,7 @@
     </row>
     <row r="399">
       <c r="A399" s="1" t="n">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B399" t="inlineStr">
         <is>
@@ -13213,7 +13213,7 @@
     </row>
     <row r="400">
       <c r="A400" s="1" t="n">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B400" t="inlineStr">
         <is>
@@ -13245,7 +13245,7 @@
     </row>
     <row r="401">
       <c r="A401" s="1" t="n">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B401" t="inlineStr">
         <is>

</xml_diff>